<commit_message>
If sheet name but not xls path specified, assume sheet is in same file
</commit_message>
<xml_diff>
--- a/excelData/cementFactory.xlsx
+++ b/excelData/cementFactory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D8011B-2686-A94B-9823-22541A1FCB99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD1D4D4-1B2F-434D-993C-210AD39AEF2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>ChainName</t>
   </si>
@@ -203,7 +203,13 @@
     <t>CO2 Capture</t>
   </si>
   <si>
-    <t>excelData/cementFactory.xlsx</t>
+    <t>here</t>
+  </si>
+  <si>
+    <t>thisfile</t>
+  </si>
+  <si>
+    <t>same</t>
   </si>
 </sst>
 </file>
@@ -578,7 +584,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,7 +592,7 @@
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -635,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -652,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
recycle flows usable at factory level
added functionality for recycle flows in factory connections table
works for 1to1 and energy_replacing_fuel as expected
ability to specify purge and maximum replacement fractions for recycles
intermediate flows appeal to calculate correctly
diagram updates directly
mass/energy dataframe sort now sorts values as well as index
intermediate flow data now returned from chain
table of internal flows now added to factory output excel
minor symbol name changes
TODO: more/updated docstrings
</commit_message>
<xml_diff>
--- a/excelData/cementFactory.xlsx
+++ b/excelData/cementFactory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD1D4D4-1B2F-434D-993C-210AD39AEF2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB701A61-3E95-9A4A-B400-BDFD9972F8C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{EAC7D76D-1E0E-F74E-87ED-1328504900CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="cementFactoryChains" localSheetId="0">'Chain List'!$A$1:$D$4</definedName>
-    <definedName name="cementFactoryConnections" localSheetId="1">Connections!$A$1:$F$4</definedName>
+    <definedName name="cementFactoryConnections" localSheetId="1">Connections!$B$1:$F$4</definedName>
     <definedName name="cementFlow" localSheetId="2">'Cement Chain'!$A$1:$C$4</definedName>
     <definedName name="CO2CapFlow" localSheetId="4">'CO2 Capture'!$A$1:$C$3</definedName>
     <definedName name="powerFlow" localSheetId="3">'Power Chain'!$A$1:$C$2</definedName>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>ChainName</t>
   </si>
@@ -128,12 +128,6 @@
     <t>ChainSheet</t>
   </si>
   <si>
-    <t>OriginChain</t>
-  </si>
-  <si>
-    <t>OriginProcess</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Product_IO_of_Destination</t>
   </si>
   <si>
-    <t>DestinationChain</t>
-  </si>
-  <si>
     <t>kiln</t>
   </si>
   <si>
@@ -210,6 +201,33 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>Recycle_Replacing</t>
+  </si>
+  <si>
+    <t>Purge_Fraction</t>
+  </si>
+  <si>
+    <t>Origin_Unit</t>
+  </si>
+  <si>
+    <t>Destination_Unit</t>
+  </si>
+  <si>
+    <t>Origin_Chain</t>
+  </si>
+  <si>
+    <t>Destination_Chain</t>
+  </si>
+  <si>
+    <t>Max_Replace_Fraction</t>
+  </si>
+  <si>
+    <t>gypsum</t>
+  </si>
+  <si>
+    <t>waste heat</t>
   </si>
 </sst>
 </file>
@@ -583,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE9E7BF-3E02-094F-9C49-4330CA199B98}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -624,10 +642,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -641,10 +659,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -658,10 +676,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -671,98 +689,173 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AFC89D-04CC-084A-B745-788782739698}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -787,43 +880,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -839,7 +932,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,21 +944,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -880,7 +973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A504ED3-B4B0-9E44-A0DD-1742FF55E35D}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -891,13 +986,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -905,21 +1000,21 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>